<commit_message>
estabilizacion de transacciones saldos por producto y data
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/bloqueos/Bloqueo.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/bloqueos/Bloqueo.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\bloqueo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486AD91F-B46A-4BF1-9CD1-CD7702A4F8FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -58,12 +52,30 @@
     <t>validarClave</t>
   </si>
   <si>
+    <t>tipoTarjeta</t>
+  </si>
+  <si>
+    <t>numeroTarjeta</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
+    <t>22483228</t>
+  </si>
+  <si>
+    <t>autouser21</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
     <t>4321</t>
   </si>
   <si>
+    <t>Acierto</t>
+  </si>
+  <si>
     <t>000</t>
   </si>
   <si>
@@ -79,34 +91,22 @@
     <t>ACTIVO</t>
   </si>
   <si>
-    <t>Acierto</t>
-  </si>
-  <si>
-    <t>tipoTarjeta</t>
-  </si>
-  <si>
-    <t>numeroTarjeta</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>autouser20</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>userrobot9</t>
   </si>
   <si>
     <t>Visa</t>
   </si>
   <si>
     <t>8337</t>
-  </si>
-  <si>
-    <t>22483228</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>userrobot9</t>
-  </si>
-  <si>
-    <t>6789</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>4</t>
@@ -115,8 +115,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,8 +145,144 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +301,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -183,35 +511,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -498,252 +1109,253 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="11.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="16.8571428571429" customWidth="1"/>
+    <col min="7" max="8" width="15.4285714285714" customWidth="1"/>
+    <col min="9" max="10" width="23.4285714285714" customWidth="1"/>
+    <col min="11" max="11" width="20.7142857142857" customWidth="1"/>
+    <col min="12" max="13" width="16.8571428571429" customWidth="1"/>
+    <col min="14" max="14" width="27.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:14">
+      <c r="A2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="I2" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="9" customFormat="1">
-      <c r="A2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="8"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="8"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>23</v>
+      <c r="M4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>23</v>
+      <c r="N5" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="M10" s="5"/>
+    <row r="10" spans="13:13">
+      <c r="M10" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" display="jalzate@todo1.net" xr:uid="{BDDEF916-466D-4BB7-91DE-68E935FB95A6}"/>
-    <hyperlink ref="N5" r:id="rId2" display="jalzate@todo1.net" xr:uid="{C3C9B005-6A77-44C8-AC72-DAE5F1E0AD86}"/>
+    <hyperlink ref="N4" r:id="rId1" display="8337"/>
+    <hyperlink ref="N5" r:id="rId1" display="8337"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
estabilización bloqueos, saldos por producto y clave dinamica
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/bloqueos/Bloqueo.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/bloqueos/Bloqueo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -94,22 +94,25 @@
     <t>2</t>
   </si>
   <si>
-    <t>autouser20</t>
+    <t>autotest13</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>userrobot9</t>
+    <t>invictus10</t>
   </si>
   <si>
     <t>Visa</t>
   </si>
   <si>
-    <t>8337</t>
+    <t>*4895</t>
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>autouser15</t>
   </si>
 </sst>
 </file>
@@ -117,12 +120,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +149,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -153,22 +164,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,11 +187,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -205,40 +256,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,31 +278,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,6 +314,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -315,49 +350,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,121 +482,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,9 +549,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,17 +573,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,37 +606,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -630,132 +641,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -764,6 +775,7 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
@@ -1118,7 +1130,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1179,22 +1191,22 @@
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:14">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1209,32 +1221,32 @@
       <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1249,32 +1261,32 @@
       <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>24</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1289,36 +1301,36 @@
       <c r="J4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1333,26 +1345,21 @@
       <c r="J5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="10" spans="13:13">
-      <c r="M10" s="8"/>
+      <c r="M10" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" display="8337"/>
-    <hyperlink ref="N5" r:id="rId1" display="8337"/>
+    <hyperlink ref="N4" r:id="rId1" display="*4895"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>